<commit_message>
Cambios en la memoria y excels
</commit_message>
<xml_diff>
--- a/Medidas/Gráfico paralelizado.xlsx
+++ b/Medidas/Gráfico paralelizado.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Desktop\Practica_Arco_OpenMP\Medidas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27D01408-1408-4CF8-A295-56E13A41347C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E42C73-9BBE-481C-A01C-AF18F15B6191}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8442DF10-1DD4-4B86-9583-3739CE60226A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Tamaño vector</t>
   </si>
@@ -53,12 +53,79 @@
   <si>
     <t>Par_Dm</t>
   </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Pendiente A</t>
+  </si>
+  <si>
+    <t>Pendiente B</t>
+  </si>
+  <si>
+    <t>Pendiente C</t>
+  </si>
+  <si>
+    <t>Pendiente D</t>
+  </si>
+  <si>
+    <t>Pendiente Dm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diferencias entre pendientes </t>
+  </si>
+  <si>
+    <t>Relaciones entre pendientes</t>
+  </si>
+  <si>
+    <t>ΔY = Y(i+1) - Y(i)</t>
+  </si>
+  <si>
+    <t>ΔX = X(i+1) - X(i)</t>
+  </si>
+  <si>
+    <t>FORMULA PEDIENTES</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>m=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Δ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Y/ΔX</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,12 +213,21 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="16"/>
       <color theme="1"/>
-      <name val="Liberation Sans"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,6 +276,12 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -246,13 +328,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -310,6 +423,806 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
+            <a:pPr lvl="1" algn="ctr" rtl="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Ejecución</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" baseline="0"/>
+              <a:t> ordenaVectorOMP.c</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="1" algn="ctr" rtl="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Par_A</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40010</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80010</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120010</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160010</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6.4333333333333353E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3551.680033333334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14501.207033333334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30867.656233333339</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56339.399733333325</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CF8F-4764-BEF9-4D05C47FC8CB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Par_B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40010</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80010</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120010</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160010</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$E$2:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.6000000000000017E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>921.7709666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3840.270766666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8545.1809999999987</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14738.589533333337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CF8F-4764-BEF9-4D05C47FC8CB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Par_C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40010</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80010</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120010</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160010</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$G$2:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.5000000000000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4075.1757999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17468.222000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39307.296866666671</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68586.341133333335</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CF8F-4764-BEF9-4D05C47FC8CB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Par_D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40010</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80010</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120010</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160010</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$I$2:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.8166666666666675E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>838.29650000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3564.9611000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8729.2836666666681</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12781.006500000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-CF8F-4764-BEF9-4D05C47FC8CB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Par_Dm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40010</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80010</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120010</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160010</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$K$2:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.1866666666666663E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1072.5238666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4956.0294999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10283.237633333332</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17283.342433333335</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-CF8F-4764-BEF9-4D05C47FC8CB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1385164975"/>
+        <c:axId val="1377323567"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1385164975"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Tamaño</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t> del vector</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1377323567"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1377323567"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Tiempo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1385164975"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -325,12 +1238,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-ES"/>
-              <a:t>Ejecución</a:t>
+              <a:t>Pendientes</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="es-ES" baseline="0"/>
-              <a:t> ordenaVectorOMP.c</a:t>
+              <a:t> ejecución ordenaVectorOMP.c</a:t>
             </a:r>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -366,25 +1280,25 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$B$1</c:f>
+              <c:f>Hoja1!$AF$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Par_A</c:v>
+                  <c:v>Pendiente A</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -393,23 +1307,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
-          <c:xVal>
+          <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$6</c:f>
+              <c:f>Hoja1!$AE$12:$AE$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -417,48 +1319,48 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>40010</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1210</c:v>
+                  <c:v>80010</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13310</c:v>
+                  <c:v>120010</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>146410</c:v>
+                  <c:v>160010</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$6</c:f>
+              <c:f>Hoja1!$AF$12:$AF$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4.223333333333338E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63.582333333333331</c:v>
+                  <c:v>8.8790392500000023E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.041333333333327</c:v>
+                  <c:v>0.27373817500000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>444.81433333333331</c:v>
+                  <c:v>0.4091612300000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46904.812666666665</c:v>
+                  <c:v>0.6367935874999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
+          </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8F2F-4017-B29D-8C583418B32C}"/>
+              <c16:uniqueId val="{00000000-8171-402D-9648-EA195E6983D3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -467,17 +1369,17 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$C$1</c:f>
+              <c:f>Hoja1!$AG$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Par_B</c:v>
+                  <c:v>Pendiente B</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -486,23 +1388,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
-          <c:xVal>
+          <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$6</c:f>
+              <c:f>Hoja1!$AE$12:$AE$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -510,48 +1400,48 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>40010</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1210</c:v>
+                  <c:v>80010</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13310</c:v>
+                  <c:v>120010</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>146410</c:v>
+                  <c:v>160010</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$2:$C$6</c:f>
+              <c:f>Hoja1!$AG$12:$AG$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.7666666666666673E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7333333333333336E-2</c:v>
+                  <c:v>2.3044159166666665E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0099999999999998</c:v>
+                  <c:v>7.2962495000000016E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>117.85133333333333</c:v>
+                  <c:v>0.1176227558333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13315.910333333331</c:v>
+                  <c:v>0.15483521333333347</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
+          </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8F2F-4017-B29D-8C583418B32C}"/>
+              <c16:uniqueId val="{00000001-8171-402D-9648-EA195E6983D3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -560,17 +1450,17 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$D$1</c:f>
+              <c:f>Hoja1!$AH$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Par_C</c:v>
+                  <c:v>Pendiente C</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -579,23 +1469,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
-          <c:xVal>
+          <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$6</c:f>
+              <c:f>Hoja1!$AE$12:$AE$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -603,48 +1481,48 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>40010</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1210</c:v>
+                  <c:v>80010</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13310</c:v>
+                  <c:v>120010</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>146410</c:v>
+                  <c:v>160010</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Hoja1!$D$2:$D$6</c:f>
+              <c:f>Hoja1!$AH$12:$AH$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.0333333333333323E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5000000000000003E-2</c:v>
+                  <c:v>0.10187925749999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5783333333333331</c:v>
+                  <c:v>0.33482615500000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>442.32266666666675</c:v>
+                  <c:v>0.54597687166666675</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>61766.065999999992</c:v>
+                  <c:v>0.73197610666666657</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
+          </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-8F2F-4017-B29D-8C583418B32C}"/>
+              <c16:uniqueId val="{00000002-8171-402D-9648-EA195E6983D3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -653,17 +1531,17 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$E$1</c:f>
+              <c:f>Hoja1!$AI$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Par_D</c:v>
+                  <c:v>Pendiente D</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -672,23 +1550,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
-          <c:xVal>
+          <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$6</c:f>
+              <c:f>Hoja1!$AE$12:$AE$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -696,48 +1562,48 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>40010</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1210</c:v>
+                  <c:v>80010</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13310</c:v>
+                  <c:v>120010</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>146410</c:v>
+                  <c:v>160010</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Hoja1!$E$2:$E$6</c:f>
+              <c:f>Hoja1!$AI$12:$AI$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.12E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19566666666666666</c:v>
+                  <c:v>2.0956458333333334E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3643333333333336</c:v>
+                  <c:v>6.8166615000000014E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>169.0453333333333</c:v>
+                  <c:v>0.1291080641666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23063.599333333335</c:v>
+                  <c:v>0.10129307083333337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
+          </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-8F2F-4017-B29D-8C583418B32C}"/>
+              <c16:uniqueId val="{00000003-8171-402D-9648-EA195E6983D3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -746,17 +1612,17 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$F$1</c:f>
+              <c:f>Hoja1!$AJ$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Par_Dm</c:v>
+                  <c:v>Pendiente Dm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
@@ -765,23 +1631,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
-          <c:xVal>
+          <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$6</c:f>
+              <c:f>Hoja1!$AE$12:$AE$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -789,48 +1643,48 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>40010</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1210</c:v>
+                  <c:v>80010</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13310</c:v>
+                  <c:v>120010</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>146410</c:v>
+                  <c:v>160010</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Hoja1!$F$2:$F$6</c:f>
+              <c:f>Hoja1!$AJ$12:$AJ$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.1399999999999992E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18999999999999997</c:v>
+                  <c:v>2.6812549999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3946666666666663</c:v>
+                  <c:v>9.7087640833333336E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>194.30033333333327</c:v>
+                  <c:v>0.1331802033333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29334.438666666672</c:v>
+                  <c:v>0.17500262000000008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
+          </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-8F2F-4017-B29D-8C583418B32C}"/>
+              <c16:uniqueId val="{00000004-8171-402D-9648-EA195E6983D3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -842,30 +1696,72 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="713587328"/>
-        <c:axId val="663731424"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="713587328"/>
+        <c:smooth val="0"/>
+        <c:axId val="1525039248"/>
+        <c:axId val="1521025728"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1525039248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Tamaño del vector</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -875,8 +1771,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -903,12 +1799,15 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="663731424"/>
+        <c:crossAx val="1521025728"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="663731424"/>
+        <c:axId val="1521025728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -928,20 +1827,69 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Valor de la pendiente</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -965,9 +1913,9 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="713587328"/>
+        <c:crossAx val="1525039248"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1085,8 +2033,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1113,8 +2101,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1194,6 +2182,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1204,6 +2197,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1215,7 +2213,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1235,6 +2233,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1247,10 +2248,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1290,23 +2291,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1411,8 +2411,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1544,12 +2544,315 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -1560,28 +2863,229 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1605,23 +3109,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1009650</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
+        <xdr:cNvPr id="5" name="Gráfico 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDAC6A21-2773-4D8E-B936-236F69B5FF44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CF5C0C0-FCDD-4FA1-8094-66AD903FE208}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1634,6 +3138,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4173C4D-04E9-4B7C-8543-499AB0F75AF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1939,138 +3479,634 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993D18EC-0970-4F95-811F-1DECD8906D4B}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:AJ54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W32" sqref="W32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:36" s="1" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="3">
+    <row r="2" spans="1:36">
+      <c r="A2" s="2">
         <v>10</v>
       </c>
-      <c r="B2" s="2">
-        <v>4.223333333333338E-2</v>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" s="2">
-        <v>2.7666666666666673E-3</v>
-      </c>
-      <c r="D2" s="2">
-        <v>3.0333333333333323E-3</v>
+        <v>6.4333333333333353E-2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E2" s="2">
-        <v>2.12E-2</v>
-      </c>
-      <c r="F2" s="2">
-        <v>2.1399999999999992E-2</v>
+        <v>4.6000000000000017E-3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2">
+        <v>5.5000000000000005E-3</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2">
+        <v>3.8166666666666675E-2</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="2">
+        <v>2.1866666666666663E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3">
-        <v>110</v>
+    <row r="3" spans="1:36">
+      <c r="A3" s="2">
+        <v>40010</v>
       </c>
       <c r="B3" s="2">
-        <v>63.582333333333331</v>
+        <f>(C3-C2)/(A3-A2)</f>
+        <v>8.8790392500000023E-2</v>
       </c>
       <c r="C3" s="2">
-        <v>1.7333333333333336E-2</v>
+        <v>3551.680033333334</v>
       </c>
       <c r="D3" s="2">
-        <v>3.5000000000000003E-2</v>
+        <f>(E3-E2)/(A3-A2)</f>
+        <v>2.3044159166666665E-2</v>
       </c>
       <c r="E3" s="2">
-        <v>0.19566666666666666</v>
+        <v>921.7709666666666</v>
       </c>
       <c r="F3" s="2">
-        <v>0.18999999999999997</v>
+        <f>(G3-G2)/(A3-A2)</f>
+        <v>0.10187925749999999</v>
+      </c>
+      <c r="G3" s="2">
+        <v>4075.1757999999995</v>
+      </c>
+      <c r="H3" s="2">
+        <f>(I3-I2)/(A3-A2)</f>
+        <v>2.0956458333333334E-2</v>
+      </c>
+      <c r="I3" s="2">
+        <v>838.29650000000004</v>
+      </c>
+      <c r="J3" s="2">
+        <f>(K3-K2)/(A3-A2)</f>
+        <v>2.6812549999999997E-2</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1072.5238666666667</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="3">
-        <v>1210</v>
+    <row r="4" spans="1:36">
+      <c r="A4" s="2">
+        <v>80010</v>
       </c>
       <c r="B4" s="2">
-        <v>34.041333333333327</v>
+        <f t="shared" ref="B4:B5" si="0">(C4-C3)/(A4-A3)</f>
+        <v>0.27373817500000003</v>
       </c>
       <c r="C4" s="2">
-        <v>1.0099999999999998</v>
+        <v>14501.207033333334</v>
       </c>
       <c r="D4" s="2">
-        <v>3.5783333333333331</v>
+        <f t="shared" ref="D4:D6" si="1">(E4-E3)/(A4-A3)</f>
+        <v>7.2962495000000016E-2</v>
       </c>
       <c r="E4" s="2">
-        <v>2.3643333333333336</v>
+        <v>3840.270766666667</v>
       </c>
       <c r="F4" s="2">
-        <v>2.3946666666666663</v>
+        <f t="shared" ref="F4:F6" si="2">(G4-G3)/(A4-A3)</f>
+        <v>0.33482615500000007</v>
+      </c>
+      <c r="G4" s="2">
+        <v>17468.222000000002</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H6" si="3">(I4-I3)/(A4-A3)</f>
+        <v>6.8166615000000014E-2</v>
+      </c>
+      <c r="I4" s="2">
+        <v>3564.9611000000004</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" ref="J4:J6" si="4">(K4-K3)/(A4-A3)</f>
+        <v>9.7087640833333336E-2</v>
+      </c>
+      <c r="K4" s="2">
+        <v>4956.0294999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3">
-        <v>13310</v>
+    <row r="5" spans="1:36">
+      <c r="A5" s="2">
+        <v>120010</v>
       </c>
       <c r="B5" s="2">
-        <v>444.81433333333331</v>
+        <f t="shared" si="0"/>
+        <v>0.4091612300000001</v>
       </c>
       <c r="C5" s="2">
-        <v>117.85133333333333</v>
+        <v>30867.656233333339</v>
       </c>
       <c r="D5" s="2">
-        <v>442.32266666666675</v>
+        <f t="shared" si="1"/>
+        <v>0.1176227558333333</v>
       </c>
       <c r="E5" s="2">
-        <v>169.0453333333333</v>
+        <v>8545.1809999999987</v>
       </c>
       <c r="F5" s="2">
-        <v>194.30033333333327</v>
+        <f t="shared" si="2"/>
+        <v>0.54597687166666675</v>
+      </c>
+      <c r="G5" s="2">
+        <v>39307.296866666671</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="3"/>
+        <v>0.1291080641666667</v>
+      </c>
+      <c r="I5" s="2">
+        <v>8729.2836666666681</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="4"/>
+        <v>0.1331802033333333</v>
+      </c>
+      <c r="K5" s="2">
+        <v>10283.237633333332</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3">
-        <v>146410</v>
+    <row r="6" spans="1:36">
+      <c r="A6" s="2">
+        <v>160010</v>
       </c>
       <c r="B6" s="2">
-        <v>46904.812666666665</v>
+        <f>(C6-C5)/(A6-A5)</f>
+        <v>0.6367935874999997</v>
       </c>
       <c r="C6" s="2">
-        <v>13315.910333333331</v>
+        <v>56339.399733333325</v>
       </c>
       <c r="D6" s="2">
-        <v>61766.065999999992</v>
+        <f t="shared" si="1"/>
+        <v>0.15483521333333347</v>
       </c>
       <c r="E6" s="2">
-        <v>23063.599333333335</v>
+        <v>14738.589533333337</v>
       </c>
       <c r="F6" s="2">
-        <v>29334.438666666672</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>0.73197610666666657</v>
+      </c>
+      <c r="G6" s="2">
+        <v>68586.341133333335</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="3"/>
+        <v>0.10129307083333337</v>
+      </c>
+      <c r="I6" s="2">
+        <v>12781.006500000003</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="4"/>
+        <v>0.17500262000000008</v>
+      </c>
+      <c r="K6" s="2">
+        <v>17283.342433333335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36">
+      <c r="A7" s="6"/>
+      <c r="B7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+    </row>
+    <row r="8" spans="1:36">
+      <c r="A8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="10">
+        <f>B4-B3</f>
+        <v>0.18494778249999999</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10">
+        <f t="shared" ref="D8:J8" si="5">D4-D3</f>
+        <v>4.9918335833333355E-2</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10">
+        <f t="shared" si="5"/>
+        <v>0.23294689750000008</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10">
+        <f t="shared" si="5"/>
+        <v>4.7210156666666683E-2</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10">
+        <f t="shared" si="5"/>
+        <v>7.0275090833333331E-2</v>
+      </c>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:36">
+      <c r="A9" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="10">
+        <f t="shared" ref="B9:J9" si="6">B5-B4</f>
+        <v>0.13542305500000007</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10">
+        <f t="shared" si="6"/>
+        <v>4.4660260833333285E-2</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10">
+        <f t="shared" si="6"/>
+        <v>0.21115071666666668</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10">
+        <f t="shared" si="6"/>
+        <v>6.0941449166666689E-2</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10">
+        <f t="shared" si="6"/>
+        <v>3.6092562499999967E-2</v>
+      </c>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:36">
+      <c r="A10" s="12"/>
+      <c r="B10" s="10">
+        <f t="shared" ref="B10:J10" si="7">B6-B5</f>
+        <v>0.2276323574999996</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10">
+        <f t="shared" si="7"/>
+        <v>3.7212457500000171E-2</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10">
+        <f t="shared" si="7"/>
+        <v>0.18599923499999982</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10">
+        <f t="shared" si="7"/>
+        <v>-2.7814993333333329E-2</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10">
+        <f t="shared" si="7"/>
+        <v>4.1822416666666778E-2</v>
+      </c>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="1:36">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="AE11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ11" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36">
+      <c r="A12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="10">
+        <f>B3/B4</f>
+        <v>0.32436247702754656</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="9">
+        <f t="shared" ref="D12:J12" si="8">D3/D4</f>
+        <v>0.31583567923035882</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9">
+        <f t="shared" si="8"/>
+        <v>0.30427508717172935</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9">
+        <f t="shared" si="8"/>
+        <v>0.30742993961682458</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9">
+        <f t="shared" si="8"/>
+        <v>0.27616851918389984</v>
+      </c>
+      <c r="K12" s="9"/>
+      <c r="AE12" s="5">
+        <v>10</v>
+      </c>
+      <c r="AF12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36">
+      <c r="A13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="10">
+        <f t="shared" ref="B13:J13" si="9">B4/B5</f>
+        <v>0.66902275907226094</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="9">
+        <f t="shared" si="9"/>
+        <v>0.62030934816205907</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9">
+        <f t="shared" si="9"/>
+        <v>0.61326069358560709</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9">
+        <f t="shared" si="9"/>
+        <v>0.52798107879615597</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9">
+        <f t="shared" si="9"/>
+        <v>0.72899453825231952</v>
+      </c>
+      <c r="K13" s="9"/>
+      <c r="AE13" s="5">
+        <v>40010</v>
+      </c>
+      <c r="AF13" s="5">
+        <v>8.8790392500000023E-2</v>
+      </c>
+      <c r="AG13" s="5">
+        <v>2.3044159166666665E-2</v>
+      </c>
+      <c r="AH13" s="5">
+        <v>0.10187925749999999</v>
+      </c>
+      <c r="AI13" s="5">
+        <v>2.0956458333333334E-2</v>
+      </c>
+      <c r="AJ13" s="5">
+        <v>2.6812549999999997E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36">
+      <c r="A14" s="8"/>
+      <c r="B14" s="10">
+        <f t="shared" ref="B14:J14" si="10">B5/B6</f>
+        <v>0.64253352739674108</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="9">
+        <f t="shared" si="10"/>
+        <v>0.75966411839477255</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9">
+        <f t="shared" si="10"/>
+        <v>0.74589439012289827</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9">
+        <f t="shared" si="10"/>
+        <v>1.2745991715376055</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9">
+        <f t="shared" si="10"/>
+        <v>0.76101833980161693</v>
+      </c>
+      <c r="K14" s="9"/>
+      <c r="AE14" s="5">
+        <v>80010</v>
+      </c>
+      <c r="AF14" s="5">
+        <v>0.27373817500000003</v>
+      </c>
+      <c r="AG14" s="5">
+        <v>7.2962495000000016E-2</v>
+      </c>
+      <c r="AH14" s="5">
+        <v>0.33482615500000007</v>
+      </c>
+      <c r="AI14" s="5">
+        <v>6.8166615000000014E-2</v>
+      </c>
+      <c r="AJ14" s="5">
+        <v>9.7087640833333336E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36">
+      <c r="AE15" s="5">
+        <v>120010</v>
+      </c>
+      <c r="AF15" s="5">
+        <v>0.4091612300000001</v>
+      </c>
+      <c r="AG15" s="5">
+        <v>0.1176227558333333</v>
+      </c>
+      <c r="AH15" s="5">
+        <v>0.54597687166666675</v>
+      </c>
+      <c r="AI15" s="5">
+        <v>0.1291080641666667</v>
+      </c>
+      <c r="AJ15" s="5">
+        <v>0.1331802033333333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36">
+      <c r="AE16" s="5">
+        <v>160010</v>
+      </c>
+      <c r="AF16" s="5">
+        <v>0.6367935874999997</v>
+      </c>
+      <c r="AG16" s="5">
+        <v>0.15483521333333347</v>
+      </c>
+      <c r="AH16" s="5">
+        <v>0.73197610666666657</v>
+      </c>
+      <c r="AI16" s="5">
+        <v>0.10129307083333337</v>
+      </c>
+      <c r="AJ16" s="5">
+        <v>0.17500262000000008</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B11:K11"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>